<commit_message>
file013 translates walls correcly
</commit_message>
<xml_diff>
--- a/RevitDynamo/12files/AllTogether.xlsx
+++ b/RevitDynamo/12files/AllTogether.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmsil\Desktop\bsp3\RevitDynamo\12files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C64B1B7-8BF0-4904-8D4A-0BA9E283C6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A6F8B6-2C03-48CE-A99A-AD2196F0BC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{79F8FA3C-B5BD-4925-A4D7-8184B102EEA1}"/>
+    <workbookView xWindow="9540" yWindow="2265" windowWidth="24810" windowHeight="15345" xr2:uid="{79F8FA3C-B5BD-4925-A4D7-8184B102EEA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Wall" sheetId="6" r:id="rId1"/>
@@ -136,28 +136,28 @@
     <t>StartPointx</t>
   </si>
   <si>
+    <t>VectorZ</t>
+  </si>
+  <si>
+    <t>0.000,</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>UnconnectedHeight</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>-1351.566,</t>
+  </si>
+  <si>
     <t>81.157,</t>
-  </si>
-  <si>
-    <t>VectorZ</t>
-  </si>
-  <si>
-    <t>0.000,</t>
-  </si>
-  <si>
-    <t>-1351.566,</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>UnconnectedHeight</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Width</t>
   </si>
 </sst>
 </file>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618ACBDD-1880-436E-8556-D2B13A8B1992}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,25 +525,25 @@
         <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
         <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J1" t="s">
         <v>30</v>
@@ -570,18 +570,18 @@
         <v>23</v>
       </c>
       <c r="R1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>1441841</v>
@@ -620,10 +620,10 @@
         <v>58</v>
       </c>
       <c r="P2">
-        <v>-0.1</v>
+        <v>-0.06</v>
       </c>
       <c r="Q2">
-        <v>-0.876</v>
+        <v>-0.998</v>
       </c>
       <c r="R2">
         <v>1354</v>

</xml_diff>